<commit_message>
upd: filtro relatorio simples (mostra acessos apoós 7:50)
</commit_message>
<xml_diff>
--- a/relatorios/relatorio_frequencia_301025.xlsx
+++ b/relatorios/relatorio_frequencia_301025.xlsx
@@ -473,7 +473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -914,7 +914,7 @@
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>TURMA: EF1802</t>
+          <t>TURMA: EF1801</t>
         </is>
       </c>
       <c r="B28" s="2" t="n"/>
@@ -944,31 +944,31 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="inlineStr">
-        <is>
-          <t>2022015300</t>
-        </is>
-      </c>
-      <c r="B30" s="4" t="inlineStr">
-        <is>
-          <t>Thiago Codeço Machado</t>
-        </is>
-      </c>
-      <c r="C30" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D30" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>3478001121</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="inlineStr">
+        <is>
+          <t>Ana Luiza de Freitas Sevidanes</t>
+        </is>
+      </c>
+      <c r="C30" s="6" t="inlineStr">
+        <is>
+          <t>CHEGOU ATRASADO</t>
+        </is>
+      </c>
+      <c r="D30" s="6" t="inlineStr">
+        <is>
+          <t>Entrada: 07:50:14</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>TURMA: EF1803</t>
+          <t>TURMA: EF1802</t>
         </is>
       </c>
       <c r="B32" s="2" t="n"/>
@@ -998,614 +998,580 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="6" t="inlineStr">
+      <c r="A34" s="4" t="inlineStr">
+        <is>
+          <t>2022015300</t>
+        </is>
+      </c>
+      <c r="B34" s="4" t="inlineStr">
+        <is>
+          <t>Thiago Codeço Machado</t>
+        </is>
+      </c>
+      <c r="C34" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D34" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>TURMA: EF1803</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="n"/>
+      <c r="C36" s="2" t="n"/>
+      <c r="D36" s="2" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="inlineStr">
+        <is>
+          <t>Matrícula</t>
+        </is>
+      </c>
+      <c r="B37" s="3" t="inlineStr">
+        <is>
+          <t>Nome do Aluno</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="inlineStr">
+        <is>
+          <t>Problema</t>
+        </is>
+      </c>
+      <c r="D37" s="3" t="inlineStr">
+        <is>
+          <t>Acesso</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="inlineStr">
         <is>
           <t>3374001121</t>
         </is>
       </c>
-      <c r="B34" s="6" t="inlineStr">
+      <c r="B38" s="6" t="inlineStr">
         <is>
           <t>Ana Luísa Caveari Vieira</t>
         </is>
       </c>
-      <c r="C34" s="6" t="inlineStr">
+      <c r="C38" s="6" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D34" s="6" t="inlineStr">
+      <c r="D38" s="6" t="inlineStr">
         <is>
           <t>Entrada: 08:23:41</t>
         </is>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="6" t="inlineStr">
+    <row r="39">
+      <c r="A39" s="6" t="inlineStr">
         <is>
           <t>2022012500</t>
         </is>
       </c>
-      <c r="B35" s="6" t="inlineStr">
+      <c r="B39" s="6" t="inlineStr">
         <is>
           <t>Serena Rocha Rangel de Sá</t>
         </is>
       </c>
-      <c r="C35" s="6" t="inlineStr">
+      <c r="C39" s="6" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D35" s="6" t="inlineStr">
+      <c r="D39" s="6" t="inlineStr">
         <is>
           <t>Entrada: 09:56:10</t>
         </is>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="2" t="inlineStr">
+    <row r="41">
+      <c r="A41" s="2" t="inlineStr">
         <is>
           <t>TURMA: EF1901</t>
         </is>
       </c>
-      <c r="B37" s="2" t="n"/>
-      <c r="C37" s="2" t="n"/>
-      <c r="D37" s="2" t="n"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="3" t="inlineStr">
+      <c r="B41" s="2" t="n"/>
+      <c r="C41" s="2" t="n"/>
+      <c r="D41" s="2" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B38" s="3" t="inlineStr">
+      <c r="B42" s="3" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C38" s="3" t="inlineStr">
+      <c r="C42" s="3" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D38" s="3" t="inlineStr">
+      <c r="D42" s="3" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="4" t="inlineStr">
+    <row r="43">
+      <c r="A43" s="4" t="inlineStr">
         <is>
           <t>3384001121</t>
         </is>
       </c>
-      <c r="B39" s="4" t="inlineStr">
+      <c r="B43" s="4" t="inlineStr">
         <is>
           <t>Antônio Marinho Calado</t>
         </is>
       </c>
-      <c r="C39" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D39" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="6" t="inlineStr">
+      <c r="C43" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D43" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6" t="inlineStr">
         <is>
           <t>2023000254</t>
         </is>
       </c>
-      <c r="B40" s="6" t="inlineStr">
+      <c r="B44" s="6" t="inlineStr">
         <is>
           <t>Bernardo Thurler da Silva</t>
         </is>
       </c>
-      <c r="C40" s="6" t="inlineStr">
+      <c r="C44" s="6" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D40" s="6" t="inlineStr">
+      <c r="D44" s="6" t="inlineStr">
         <is>
           <t>Entrada: 10:06:04</t>
         </is>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="6" t="inlineStr">
+    <row r="45">
+      <c r="A45" s="6" t="inlineStr">
         <is>
           <t>3722001122</t>
         </is>
       </c>
-      <c r="B41" s="6" t="inlineStr">
+      <c r="B45" s="6" t="inlineStr">
         <is>
           <t>Maria Eduarda Alves Hipólito</t>
         </is>
       </c>
-      <c r="C41" s="6" t="inlineStr">
+      <c r="C45" s="6" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D41" s="6" t="inlineStr">
+      <c r="D45" s="6" t="inlineStr">
         <is>
           <t>Entrada: 08:35:13</t>
         </is>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="4" t="inlineStr">
+    <row r="46">
+      <c r="A46" s="4" t="inlineStr">
         <is>
           <t>2269001115</t>
         </is>
       </c>
-      <c r="B42" s="4" t="inlineStr">
+      <c r="B46" s="4" t="inlineStr">
         <is>
           <t>Pedro Henrique Pinto Siqueira</t>
         </is>
       </c>
-      <c r="C42" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D42" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="2" t="inlineStr">
+      <c r="C46" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D46" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
         <is>
           <t>TURMA: EM2101</t>
         </is>
       </c>
-      <c r="B44" s="2" t="n"/>
-      <c r="C44" s="2" t="n"/>
-      <c r="D44" s="2" t="n"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="3" t="inlineStr">
+      <c r="B48" s="2" t="n"/>
+      <c r="C48" s="2" t="n"/>
+      <c r="D48" s="2" t="n"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B45" s="3" t="inlineStr">
+      <c r="B49" s="3" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C45" s="3" t="inlineStr">
+      <c r="C49" s="3" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D45" s="3" t="inlineStr">
+      <c r="D49" s="3" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="6" t="inlineStr">
+    <row r="50">
+      <c r="A50" s="6" t="inlineStr">
         <is>
           <t>2025000593</t>
         </is>
       </c>
-      <c r="B46" s="6" t="inlineStr">
+      <c r="B50" s="6" t="inlineStr">
         <is>
           <t>Bernardo de Castro Ribeiro</t>
         </is>
       </c>
-      <c r="C46" s="6" t="inlineStr">
+      <c r="C50" s="6" t="inlineStr">
         <is>
           <t>CHEGOU ATRASADO</t>
         </is>
       </c>
-      <c r="D46" s="6" t="inlineStr">
+      <c r="D50" s="6" t="inlineStr">
         <is>
           <t>Entrada: 08:54:13</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="4" t="inlineStr">
-        <is>
-          <t>2025000573</t>
-        </is>
-      </c>
-      <c r="B47" s="4" t="inlineStr">
-        <is>
-          <t>Luma de Oliveira Carvalho</t>
-        </is>
-      </c>
-      <c r="C47" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D47" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="2" t="inlineStr">
-        <is>
-          <t>TURMA: EM2201</t>
-        </is>
-      </c>
-      <c r="B49" s="2" t="n"/>
-      <c r="C49" s="2" t="n"/>
-      <c r="D49" s="2" t="n"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="3" t="inlineStr">
-        <is>
-          <t>Matrícula</t>
-        </is>
-      </c>
-      <c r="B50" s="3" t="inlineStr">
-        <is>
-          <t>Nome do Aluno</t>
-        </is>
-      </c>
-      <c r="C50" s="3" t="inlineStr">
-        <is>
-          <t>Problema</t>
-        </is>
-      </c>
-      <c r="D50" s="3" t="inlineStr">
-        <is>
-          <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="4" t="inlineStr">
         <is>
+          <t>2025000573</t>
+        </is>
+      </c>
+      <c r="B51" s="4" t="inlineStr">
+        <is>
+          <t>Luma de Oliveira Carvalho</t>
+        </is>
+      </c>
+      <c r="C51" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D51" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="inlineStr">
+        <is>
+          <t>TURMA: EM2201</t>
+        </is>
+      </c>
+      <c r="B53" s="2" t="n"/>
+      <c r="C53" s="2" t="n"/>
+      <c r="D53" s="2" t="n"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="inlineStr">
+        <is>
+          <t>Matrícula</t>
+        </is>
+      </c>
+      <c r="B54" s="3" t="inlineStr">
+        <is>
+          <t>Nome do Aluno</t>
+        </is>
+      </c>
+      <c r="C54" s="3" t="inlineStr">
+        <is>
+          <t>Problema</t>
+        </is>
+      </c>
+      <c r="D54" s="3" t="inlineStr">
+        <is>
+          <t>Acesso</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="inlineStr">
+        <is>
           <t>2024000467</t>
         </is>
       </c>
-      <c r="B51" s="4" t="inlineStr">
+      <c r="B55" s="4" t="inlineStr">
         <is>
           <t>Isabel Batista Moura</t>
         </is>
       </c>
-      <c r="C51" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D51" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="4" t="inlineStr">
+      <c r="C55" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D55" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="inlineStr">
         <is>
           <t>2024000512</t>
         </is>
       </c>
-      <c r="B52" s="4" t="inlineStr">
+      <c r="B56" s="4" t="inlineStr">
         <is>
           <t>Rebeca de Paula Machado</t>
         </is>
       </c>
-      <c r="C52" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D52" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="2" t="inlineStr">
+      <c r="C56" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D56" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="inlineStr">
         <is>
           <t>TURMA: EM2202</t>
         </is>
       </c>
-      <c r="B54" s="2" t="n"/>
-      <c r="C54" s="2" t="n"/>
-      <c r="D54" s="2" t="n"/>
-    </row>
-    <row r="55">
-      <c r="A55" s="3" t="inlineStr">
+      <c r="B58" s="2" t="n"/>
+      <c r="C58" s="2" t="n"/>
+      <c r="D58" s="2" t="n"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B55" s="3" t="inlineStr">
+      <c r="B59" s="3" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C55" s="3" t="inlineStr">
+      <c r="C59" s="3" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D55" s="3" t="inlineStr">
+      <c r="D59" s="3" t="inlineStr">
         <is>
           <t>Acesso</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="5" t="inlineStr">
-        <is>
-          <t>2025000727</t>
-        </is>
-      </c>
-      <c r="B56" s="5" t="inlineStr">
-        <is>
-          <t>Arthur Cerqueira Lacerda</t>
-        </is>
-      </c>
-      <c r="C56" s="5" t="inlineStr">
-        <is>
-          <t>SAIU CEDO</t>
-        </is>
-      </c>
-      <c r="D56" s="5" t="inlineStr">
-        <is>
-          <t>Saída: 10:39:41</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="5" t="inlineStr">
-        <is>
-          <t>2024000261</t>
-        </is>
-      </c>
-      <c r="B57" s="5" t="inlineStr">
-        <is>
-          <t>Cauã Baião Guimarães Silveira e Silva</t>
-        </is>
-      </c>
-      <c r="C57" s="5" t="inlineStr">
-        <is>
-          <t>SAIU CEDO</t>
-        </is>
-      </c>
-      <c r="D57" s="5" t="inlineStr">
-        <is>
-          <t>Saída: 10:39:45</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="6" t="inlineStr">
-        <is>
-          <t>2024000296</t>
-        </is>
-      </c>
-      <c r="B58" s="6" t="inlineStr">
-        <is>
-          <t>Lara Vasconcelos Souza Ferreira Lima</t>
-        </is>
-      </c>
-      <c r="C58" s="6" t="inlineStr">
-        <is>
-          <t>CHEGOU ATRASADO</t>
-        </is>
-      </c>
-      <c r="D58" s="6" t="inlineStr">
-        <is>
-          <t>Entrada: 08:41:50</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="5" t="inlineStr">
-        <is>
-          <t>2024000468</t>
-        </is>
-      </c>
-      <c r="B59" s="5" t="inlineStr">
-        <is>
-          <t>Maria Luisa Silveira Nunes</t>
-        </is>
-      </c>
-      <c r="C59" s="5" t="inlineStr">
-        <is>
-          <t>SAIU CEDO</t>
-        </is>
-      </c>
-      <c r="D59" s="5" t="inlineStr">
-        <is>
-          <t>Saída: 10:15:25</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="inlineStr">
         <is>
+          <t>2025000727</t>
+        </is>
+      </c>
+      <c r="B60" s="5" t="inlineStr">
+        <is>
+          <t>Arthur Cerqueira Lacerda</t>
+        </is>
+      </c>
+      <c r="C60" s="5" t="inlineStr">
+        <is>
+          <t>SAIU CEDO</t>
+        </is>
+      </c>
+      <c r="D60" s="5" t="inlineStr">
+        <is>
+          <t>Saída: 10:39:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="5" t="inlineStr">
+        <is>
+          <t>2024000261</t>
+        </is>
+      </c>
+      <c r="B61" s="5" t="inlineStr">
+        <is>
+          <t>Cauã Baião Guimarães Silveira e Silva</t>
+        </is>
+      </c>
+      <c r="C61" s="5" t="inlineStr">
+        <is>
+          <t>SAIU CEDO</t>
+        </is>
+      </c>
+      <c r="D61" s="5" t="inlineStr">
+        <is>
+          <t>Saída: 10:39:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="6" t="inlineStr">
+        <is>
+          <t>2024000296</t>
+        </is>
+      </c>
+      <c r="B62" s="6" t="inlineStr">
+        <is>
+          <t>Lara Vasconcelos Souza Ferreira Lima</t>
+        </is>
+      </c>
+      <c r="C62" s="6" t="inlineStr">
+        <is>
+          <t>CHEGOU ATRASADO</t>
+        </is>
+      </c>
+      <c r="D62" s="6" t="inlineStr">
+        <is>
+          <t>Entrada: 08:41:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="5" t="inlineStr">
+        <is>
+          <t>2024000468</t>
+        </is>
+      </c>
+      <c r="B63" s="5" t="inlineStr">
+        <is>
+          <t>Maria Luisa Silveira Nunes</t>
+        </is>
+      </c>
+      <c r="C63" s="5" t="inlineStr">
+        <is>
+          <t>SAIU CEDO</t>
+        </is>
+      </c>
+      <c r="D63" s="5" t="inlineStr">
+        <is>
+          <t>Saída: 10:15:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="5" t="inlineStr">
+        <is>
           <t>2024000289</t>
         </is>
       </c>
-      <c r="B60" s="5" t="inlineStr">
+      <c r="B64" s="5" t="inlineStr">
         <is>
           <t>Ricardo de Almeida Nunes Pessanha</t>
         </is>
       </c>
-      <c r="C60" s="5" t="inlineStr">
+      <c r="C64" s="5" t="inlineStr">
         <is>
           <t>SAIU CEDO</t>
         </is>
       </c>
-      <c r="D60" s="5" t="inlineStr">
+      <c r="D64" s="5" t="inlineStr">
         <is>
           <t>Saída: 10:39:10</t>
         </is>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" s="2" t="inlineStr">
+    <row r="66">
+      <c r="A66" s="2" t="inlineStr">
         <is>
           <t>TURMA: EM2301</t>
         </is>
       </c>
-      <c r="B62" s="2" t="n"/>
-      <c r="C62" s="2" t="n"/>
-      <c r="D62" s="2" t="n"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="3" t="inlineStr">
+      <c r="B66" s="2" t="n"/>
+      <c r="C66" s="2" t="n"/>
+      <c r="D66" s="2" t="n"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="3" t="inlineStr">
         <is>
           <t>Matrícula</t>
         </is>
       </c>
-      <c r="B63" s="3" t="inlineStr">
+      <c r="B67" s="3" t="inlineStr">
         <is>
           <t>Nome do Aluno</t>
         </is>
       </c>
-      <c r="C63" s="3" t="inlineStr">
+      <c r="C67" s="3" t="inlineStr">
         <is>
           <t>Problema</t>
         </is>
       </c>
-      <c r="D63" s="3" t="inlineStr">
+      <c r="D67" s="3" t="inlineStr">
         <is>
           <t>Acesso</t>
         </is>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" s="4" t="inlineStr">
+    <row r="68">
+      <c r="A68" s="4" t="inlineStr">
         <is>
           <t>2023000163</t>
         </is>
       </c>
-      <c r="B64" s="4" t="inlineStr">
+      <c r="B68" s="4" t="inlineStr">
         <is>
           <t>Ana Clara Pereira Pimentel de Souza</t>
         </is>
       </c>
-      <c r="C64" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D64" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="4" t="inlineStr">
-        <is>
-          <t>2023000031</t>
-        </is>
-      </c>
-      <c r="B65" s="4" t="inlineStr">
-        <is>
-          <t>Antonella Tavares Soares</t>
-        </is>
-      </c>
-      <c r="C65" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D65" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="4" t="inlineStr">
-        <is>
-          <t>2023000174</t>
-        </is>
-      </c>
-      <c r="B66" s="4" t="inlineStr">
-        <is>
-          <t>Bruno de Oliveira Vieira</t>
-        </is>
-      </c>
-      <c r="C66" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D66" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="5" t="inlineStr">
-        <is>
-          <t>2023000034</t>
-        </is>
-      </c>
-      <c r="B67" s="5" t="inlineStr">
-        <is>
-          <t>Clara Cunha Bastos Rocha</t>
-        </is>
-      </c>
-      <c r="C67" s="5" t="inlineStr">
-        <is>
-          <t>SAIU CEDO</t>
-        </is>
-      </c>
-      <c r="D67" s="5" t="inlineStr">
-        <is>
-          <t>Saída: 09:56:46</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="5" t="inlineStr">
-        <is>
-          <t>2023000157</t>
-        </is>
-      </c>
-      <c r="B68" s="5" t="inlineStr">
-        <is>
-          <t>Clara Cunha Castro</t>
-        </is>
-      </c>
-      <c r="C68" s="5" t="inlineStr">
-        <is>
-          <t>SAIU CEDO</t>
-        </is>
-      </c>
-      <c r="D68" s="5" t="inlineStr">
-        <is>
-          <t>Saída: 10:53:03</t>
+      <c r="C68" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D68" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="4" t="inlineStr">
         <is>
-          <t>2023000035</t>
+          <t>2023000031</t>
         </is>
       </c>
       <c r="B69" s="4" t="inlineStr">
         <is>
-          <t>Davi Meirelles de Freitas</t>
+          <t>Antonella Tavares Soares</t>
         </is>
       </c>
       <c r="C69" s="4" t="inlineStr">
@@ -1622,12 +1588,12 @@
     <row r="70">
       <c r="A70" s="4" t="inlineStr">
         <is>
-          <t>2023000036</t>
+          <t>2023000174</t>
         </is>
       </c>
       <c r="B70" s="4" t="inlineStr">
         <is>
-          <t>Davi Moraes Bussade de Almeida</t>
+          <t>Bruno de Oliveira Vieira</t>
         </is>
       </c>
       <c r="C70" s="4" t="inlineStr">
@@ -1642,58 +1608,58 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="4" t="inlineStr">
-        <is>
-          <t>2024000256</t>
-        </is>
-      </c>
-      <c r="B71" s="4" t="inlineStr">
-        <is>
-          <t>Eduarda Lima Ferreira</t>
-        </is>
-      </c>
-      <c r="C71" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D71" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
+      <c r="A71" s="5" t="inlineStr">
+        <is>
+          <t>2023000034</t>
+        </is>
+      </c>
+      <c r="B71" s="5" t="inlineStr">
+        <is>
+          <t>Clara Cunha Bastos Rocha</t>
+        </is>
+      </c>
+      <c r="C71" s="5" t="inlineStr">
+        <is>
+          <t>SAIU CEDO</t>
+        </is>
+      </c>
+      <c r="D71" s="5" t="inlineStr">
+        <is>
+          <t>Saída: 09:56:46</t>
         </is>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="4" t="inlineStr">
-        <is>
-          <t>2023000155</t>
-        </is>
-      </c>
-      <c r="B72" s="4" t="inlineStr">
-        <is>
-          <t>Felipe Evaristo da Silva Marcolongo</t>
-        </is>
-      </c>
-      <c r="C72" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D72" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
+      <c r="A72" s="5" t="inlineStr">
+        <is>
+          <t>2023000157</t>
+        </is>
+      </c>
+      <c r="B72" s="5" t="inlineStr">
+        <is>
+          <t>Clara Cunha Castro</t>
+        </is>
+      </c>
+      <c r="C72" s="5" t="inlineStr">
+        <is>
+          <t>SAIU CEDO</t>
+        </is>
+      </c>
+      <c r="D72" s="5" t="inlineStr">
+        <is>
+          <t>Saída: 10:53:03</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="4" t="inlineStr">
         <is>
-          <t>2023000040</t>
+          <t>2023000035</t>
         </is>
       </c>
       <c r="B73" s="4" t="inlineStr">
         <is>
-          <t>Gabriel Moraes Moreira</t>
+          <t>Davi Meirelles de Freitas</t>
         </is>
       </c>
       <c r="C73" s="4" t="inlineStr">
@@ -1710,12 +1676,12 @@
     <row r="74">
       <c r="A74" s="4" t="inlineStr">
         <is>
-          <t>2023000041</t>
+          <t>2023000036</t>
         </is>
       </c>
       <c r="B74" s="4" t="inlineStr">
         <is>
-          <t>Giovanna Lopes Medina</t>
+          <t>Davi Moraes Bussade de Almeida</t>
         </is>
       </c>
       <c r="C74" s="4" t="inlineStr">
@@ -1732,12 +1698,12 @@
     <row r="75">
       <c r="A75" s="4" t="inlineStr">
         <is>
-          <t>2023000052</t>
+          <t>2024000256</t>
         </is>
       </c>
       <c r="B75" s="4" t="inlineStr">
         <is>
-          <t>João Pedro Mançano Bastos da Cruz</t>
+          <t>Eduarda Lima Ferreira</t>
         </is>
       </c>
       <c r="C75" s="4" t="inlineStr">
@@ -1754,12 +1720,12 @@
     <row r="76">
       <c r="A76" s="4" t="inlineStr">
         <is>
-          <t>2023000056</t>
+          <t>2023000155</t>
         </is>
       </c>
       <c r="B76" s="4" t="inlineStr">
         <is>
-          <t>Leon Fontoura Gonçalves</t>
+          <t>Felipe Evaristo da Silva Marcolongo</t>
         </is>
       </c>
       <c r="C76" s="4" t="inlineStr">
@@ -1776,12 +1742,12 @@
     <row r="77">
       <c r="A77" s="4" t="inlineStr">
         <is>
-          <t>2023000151</t>
+          <t>2023000040</t>
         </is>
       </c>
       <c r="B77" s="4" t="inlineStr">
         <is>
-          <t>Luísa Lopes de Souza</t>
+          <t>Gabriel Moraes Moreira</t>
         </is>
       </c>
       <c r="C77" s="4" t="inlineStr">
@@ -1798,12 +1764,12 @@
     <row r="78">
       <c r="A78" s="4" t="inlineStr">
         <is>
-          <t>2023000060</t>
+          <t>2023000041</t>
         </is>
       </c>
       <c r="B78" s="4" t="inlineStr">
         <is>
-          <t>Luíza Arantes Rangel Muniz</t>
+          <t>Giovanna Lopes Medina</t>
         </is>
       </c>
       <c r="C78" s="4" t="inlineStr">
@@ -1820,12 +1786,12 @@
     <row r="79">
       <c r="A79" s="4" t="inlineStr">
         <is>
-          <t>2024000504</t>
+          <t>2023000052</t>
         </is>
       </c>
       <c r="B79" s="4" t="inlineStr">
         <is>
-          <t>Murilo Kunze Soares</t>
+          <t>João Pedro Mançano Bastos da Cruz</t>
         </is>
       </c>
       <c r="C79" s="4" t="inlineStr">
@@ -1842,12 +1808,12 @@
     <row r="80">
       <c r="A80" s="4" t="inlineStr">
         <is>
-          <t>2023000202</t>
+          <t>2023000056</t>
         </is>
       </c>
       <c r="B80" s="4" t="inlineStr">
         <is>
-          <t>Patrícia Resende Rodrigues da Silva</t>
+          <t>Leon Fontoura Gonçalves</t>
         </is>
       </c>
       <c r="C80" s="4" t="inlineStr">
@@ -1864,12 +1830,12 @@
     <row r="81">
       <c r="A81" s="4" t="inlineStr">
         <is>
-          <t>2023000073</t>
+          <t>2023000151</t>
         </is>
       </c>
       <c r="B81" s="4" t="inlineStr">
         <is>
-          <t>Pedro Vardieri Monteiro de Barros</t>
+          <t>Luísa Lopes de Souza</t>
         </is>
       </c>
       <c r="C81" s="4" t="inlineStr">
@@ -1883,47 +1849,81 @@
         </is>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" s="4" t="inlineStr">
+        <is>
+          <t>2023000060</t>
+        </is>
+      </c>
+      <c r="B82" s="4" t="inlineStr">
+        <is>
+          <t>Luíza Arantes Rangel Muniz</t>
+        </is>
+      </c>
+      <c r="C82" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D82" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
     <row r="83">
-      <c r="A83" s="2" t="inlineStr">
-        <is>
-          <t>TURMA: EM2302</t>
-        </is>
-      </c>
-      <c r="B83" s="2" t="n"/>
-      <c r="C83" s="2" t="n"/>
-      <c r="D83" s="2" t="n"/>
+      <c r="A83" s="4" t="inlineStr">
+        <is>
+          <t>2024000504</t>
+        </is>
+      </c>
+      <c r="B83" s="4" t="inlineStr">
+        <is>
+          <t>Murilo Kunze Soares</t>
+        </is>
+      </c>
+      <c r="C83" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D83" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
     </row>
     <row r="84">
-      <c r="A84" s="3" t="inlineStr">
-        <is>
-          <t>Matrícula</t>
-        </is>
-      </c>
-      <c r="B84" s="3" t="inlineStr">
-        <is>
-          <t>Nome do Aluno</t>
-        </is>
-      </c>
-      <c r="C84" s="3" t="inlineStr">
-        <is>
-          <t>Problema</t>
-        </is>
-      </c>
-      <c r="D84" s="3" t="inlineStr">
-        <is>
-          <t>Acesso</t>
+      <c r="A84" s="4" t="inlineStr">
+        <is>
+          <t>2023000202</t>
+        </is>
+      </c>
+      <c r="B84" s="4" t="inlineStr">
+        <is>
+          <t>Patrícia Resende Rodrigues da Silva</t>
+        </is>
+      </c>
+      <c r="C84" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D84" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="4" t="inlineStr">
         <is>
-          <t>2023000028</t>
+          <t>2023000073</t>
         </is>
       </c>
       <c r="B85" s="4" t="inlineStr">
         <is>
-          <t>Alice Pereira Baptista</t>
+          <t>Pedro Vardieri Monteiro de Barros</t>
         </is>
       </c>
       <c r="C85" s="4" t="inlineStr">
@@ -1937,81 +1937,47 @@
         </is>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" s="4" t="inlineStr">
-        <is>
-          <t>2023000168</t>
-        </is>
-      </c>
-      <c r="B86" s="4" t="inlineStr">
-        <is>
-          <t>Ana Luísa Petterman Galito</t>
-        </is>
-      </c>
-      <c r="C86" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D86" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
     <row r="87">
-      <c r="A87" s="4" t="inlineStr">
-        <is>
-          <t>2023000033</t>
-        </is>
-      </c>
-      <c r="B87" s="4" t="inlineStr">
-        <is>
-          <t>Carolina Rodrigues de Britto</t>
-        </is>
-      </c>
-      <c r="C87" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D87" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
+      <c r="A87" s="2" t="inlineStr">
+        <is>
+          <t>TURMA: EM2302</t>
+        </is>
+      </c>
+      <c r="B87" s="2" t="n"/>
+      <c r="C87" s="2" t="n"/>
+      <c r="D87" s="2" t="n"/>
     </row>
     <row r="88">
-      <c r="A88" s="4" t="inlineStr">
-        <is>
-          <t>2023000039</t>
-        </is>
-      </c>
-      <c r="B88" s="4" t="inlineStr">
-        <is>
-          <t>Diana Alves Fortuna Pussiareli</t>
-        </is>
-      </c>
-      <c r="C88" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D88" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
+      <c r="A88" s="3" t="inlineStr">
+        <is>
+          <t>Matrícula</t>
+        </is>
+      </c>
+      <c r="B88" s="3" t="inlineStr">
+        <is>
+          <t>Nome do Aluno</t>
+        </is>
+      </c>
+      <c r="C88" s="3" t="inlineStr">
+        <is>
+          <t>Problema</t>
+        </is>
+      </c>
+      <c r="D88" s="3" t="inlineStr">
+        <is>
+          <t>Acesso</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="4" t="inlineStr">
         <is>
-          <t>2023000145</t>
+          <t>2023000028</t>
         </is>
       </c>
       <c r="B89" s="4" t="inlineStr">
         <is>
-          <t>Décio Macedo Netto</t>
+          <t>Alice Pereira Baptista</t>
         </is>
       </c>
       <c r="C89" s="4" t="inlineStr">
@@ -2028,12 +1994,12 @@
     <row r="90">
       <c r="A90" s="4" t="inlineStr">
         <is>
-          <t>2023000042</t>
+          <t>2023000168</t>
         </is>
       </c>
       <c r="B90" s="4" t="inlineStr">
         <is>
-          <t>Giovana Souza Ângelo Leite</t>
+          <t>Ana Luísa Petterman Galito</t>
         </is>
       </c>
       <c r="C90" s="4" t="inlineStr">
@@ -2050,12 +2016,12 @@
     <row r="91">
       <c r="A91" s="4" t="inlineStr">
         <is>
-          <t>2023000046</t>
+          <t>2023000033</t>
         </is>
       </c>
       <c r="B91" s="4" t="inlineStr">
         <is>
-          <t>Guilherme de Oliveira Avelino</t>
+          <t>Carolina Rodrigues de Britto</t>
         </is>
       </c>
       <c r="C91" s="4" t="inlineStr">
@@ -2072,12 +2038,12 @@
     <row r="92">
       <c r="A92" s="4" t="inlineStr">
         <is>
-          <t>2023000043</t>
+          <t>2023000039</t>
         </is>
       </c>
       <c r="B92" s="4" t="inlineStr">
         <is>
-          <t>Gustavo Martins Moura Cruz</t>
+          <t>Diana Alves Fortuna Pussiareli</t>
         </is>
       </c>
       <c r="C92" s="4" t="inlineStr">
@@ -2094,12 +2060,12 @@
     <row r="93">
       <c r="A93" s="4" t="inlineStr">
         <is>
-          <t>2023000166</t>
+          <t>2023000145</t>
         </is>
       </c>
       <c r="B93" s="4" t="inlineStr">
         <is>
-          <t>Lícia Tinoco Dias</t>
+          <t>Décio Macedo Netto</t>
         </is>
       </c>
       <c r="C93" s="4" t="inlineStr">
@@ -2116,12 +2082,12 @@
     <row r="94">
       <c r="A94" s="4" t="inlineStr">
         <is>
-          <t>2023000160</t>
+          <t>2023000042</t>
         </is>
       </c>
       <c r="B94" s="4" t="inlineStr">
         <is>
-          <t>Manuela da Silveira Lestayo</t>
+          <t>Giovana Souza Ângelo Leite</t>
         </is>
       </c>
       <c r="C94" s="4" t="inlineStr">
@@ -2138,12 +2104,12 @@
     <row r="95">
       <c r="A95" s="4" t="inlineStr">
         <is>
-          <t>2023000062</t>
+          <t>2023000046</t>
         </is>
       </c>
       <c r="B95" s="4" t="inlineStr">
         <is>
-          <t>Maria Antonia Almeida de Mattos</t>
+          <t>Guilherme de Oliveira Avelino</t>
         </is>
       </c>
       <c r="C95" s="4" t="inlineStr">
@@ -2160,12 +2126,12 @@
     <row r="96">
       <c r="A96" s="4" t="inlineStr">
         <is>
-          <t>2023000063</t>
+          <t>2023000043</t>
         </is>
       </c>
       <c r="B96" s="4" t="inlineStr">
         <is>
-          <t>Maria Júlia Faria de Souza Botelho</t>
+          <t>Gustavo Martins Moura Cruz</t>
         </is>
       </c>
       <c r="C96" s="4" t="inlineStr">
@@ -2180,36 +2146,36 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="5" t="inlineStr">
-        <is>
-          <t>2024000482</t>
-        </is>
-      </c>
-      <c r="B97" s="5" t="inlineStr">
-        <is>
-          <t>Natália Costa de Castro</t>
-        </is>
-      </c>
-      <c r="C97" s="5" t="inlineStr">
-        <is>
-          <t>SAIU CEDO</t>
-        </is>
-      </c>
-      <c r="D97" s="5" t="inlineStr">
-        <is>
-          <t>Saída: 11:22:32</t>
+      <c r="A97" s="4" t="inlineStr">
+        <is>
+          <t>2023000166</t>
+        </is>
+      </c>
+      <c r="B97" s="4" t="inlineStr">
+        <is>
+          <t>Lícia Tinoco Dias</t>
+        </is>
+      </c>
+      <c r="C97" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D97" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="4" t="inlineStr">
         <is>
-          <t>2023000177</t>
+          <t>2023000160</t>
         </is>
       </c>
       <c r="B98" s="4" t="inlineStr">
         <is>
-          <t>Rachell Almeida Heymann</t>
+          <t>Manuela da Silveira Lestayo</t>
         </is>
       </c>
       <c r="C98" s="4" t="inlineStr">
@@ -2226,12 +2192,12 @@
     <row r="99">
       <c r="A99" s="4" t="inlineStr">
         <is>
-          <t>2023000075</t>
+          <t>2023000062</t>
         </is>
       </c>
       <c r="B99" s="4" t="inlineStr">
         <is>
-          <t>Raphaela Crespo Bastos</t>
+          <t>Maria Antonia Almeida de Mattos</t>
         </is>
       </c>
       <c r="C99" s="4" t="inlineStr">
@@ -2248,62 +2214,151 @@
     <row r="100">
       <c r="A100" s="4" t="inlineStr">
         <is>
+          <t>2023000063</t>
+        </is>
+      </c>
+      <c r="B100" s="4" t="inlineStr">
+        <is>
+          <t>Maria Júlia Faria de Souza Botelho</t>
+        </is>
+      </c>
+      <c r="C100" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D100" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="5" t="inlineStr">
+        <is>
+          <t>2024000482</t>
+        </is>
+      </c>
+      <c r="B101" s="5" t="inlineStr">
+        <is>
+          <t>Natália Costa de Castro</t>
+        </is>
+      </c>
+      <c r="C101" s="5" t="inlineStr">
+        <is>
+          <t>SAIU CEDO</t>
+        </is>
+      </c>
+      <c r="D101" s="5" t="inlineStr">
+        <is>
+          <t>Saída: 11:22:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="4" t="inlineStr">
+        <is>
+          <t>2023000177</t>
+        </is>
+      </c>
+      <c r="B102" s="4" t="inlineStr">
+        <is>
+          <t>Rachell Almeida Heymann</t>
+        </is>
+      </c>
+      <c r="C102" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D102" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="4" t="inlineStr">
+        <is>
+          <t>2023000075</t>
+        </is>
+      </c>
+      <c r="B103" s="4" t="inlineStr">
+        <is>
+          <t>Raphaela Crespo Bastos</t>
+        </is>
+      </c>
+      <c r="C103" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D103" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="4" t="inlineStr">
+        <is>
           <t>2023000076</t>
         </is>
       </c>
-      <c r="B100" s="4" t="inlineStr">
+      <c r="B104" s="4" t="inlineStr">
         <is>
           <t>Ray da Silva Martins Bizarro</t>
         </is>
       </c>
-      <c r="C100" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D100" s="4" t="inlineStr">
-        <is>
-          <t>Sem registro</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="4" t="inlineStr">
+      <c r="C104" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D104" s="4" t="inlineStr">
+        <is>
+          <t>Sem registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="4" t="inlineStr">
         <is>
           <t>2025000758</t>
         </is>
       </c>
-      <c r="B101" s="4" t="inlineStr">
+      <c r="B105" s="4" t="inlineStr">
         <is>
           <t>Víctor Machado Perusso de Souza</t>
         </is>
       </c>
-      <c r="C101" s="4" t="inlineStr">
-        <is>
-          <t>FALTOU</t>
-        </is>
-      </c>
-      <c r="D101" s="4" t="inlineStr">
+      <c r="C105" s="4" t="inlineStr">
+        <is>
+          <t>FALTOU</t>
+        </is>
+      </c>
+      <c r="D105" s="4" t="inlineStr">
         <is>
           <t>Sem registro</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A58:D58"/>
     <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A48:D48"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="A41:D41"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A66:D66"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>